<commit_message>
amount feature added in dues, provision to not have duplicate entries in Due and format changes+some changes to ensure integrity of db
</commit_message>
<xml_diff>
--- a/store/himgiri.xlsx
+++ b/store/himgiri.xlsx
@@ -11,16 +11,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>Roll number</t>
   </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>20bcs001</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -32,13 +38,23 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -47,12 +63,15 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -274,31 +293,73 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1">
         <v>185001.0</v>
       </c>
+      <c r="B2" s="1">
+        <v>11.0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1">
         <v>185002.0</v>
       </c>
+      <c r="B3" s="1">
+        <v>12.0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1">
         <v>195003.0</v>
       </c>
+      <c r="B4" s="1">
+        <v>13.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1">
         <v>195004.0</v>
       </c>
+      <c r="B5" s="1">
+        <v>15.0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1">
         <v>195005.0</v>
       </c>
+      <c r="B6" s="1">
+        <v>25.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>